<commit_message>
worked more on warning messages
</commit_message>
<xml_diff>
--- a/data/example_data/ten_obs_missing_vals.xlsx
+++ b/data/example_data/ten_obs_missing_vals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegoode/Desktop/carp-rf/shiny-app/app/data/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FA6202-023E-784C-A95D-3D55BF488B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A51EDE8-0A72-0A42-A041-FAA4ECEB616D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{2C8DB93F-ED8E-D240-B60C-7DE03C7D2E86}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,9 +849,6 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
       <c r="B9" s="1">
         <v>2015</v>
       </c>

</xml_diff>

<commit_message>
finished warning and error messages (at least for now)
</commit_message>
<xml_diff>
--- a/data/example_data/ten_obs_missing_vals.xlsx
+++ b/data/example_data/ten_obs_missing_vals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegoode/Desktop/carp-rf/shiny-app/app/data/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A51EDE8-0A72-0A42-A041-FAA4ECEB616D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DECFB2F-647F-E746-80CD-2ED90669D732}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{2C8DB93F-ED8E-D240-B60C-7DE03C7D2E86}"/>
   </bookViews>
@@ -849,6 +849,9 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" s="1">
         <v>2015</v>
       </c>

</xml_diff>